<commit_message>
Add example how to transform Excel to Markdown
</commit_message>
<xml_diff>
--- a/site/sample/excel/test-multiple-sheets.xlsx
+++ b/site/sample/excel/test-multiple-sheets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgoeschl/work/github/sgoeschl/freemarker-cli/site/sample/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826402EA-E41F-1C4C-8966-0146C43AA694}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C05E932-DD01-7942-9793-7F2A9976F51D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Text</t>
   </si>
@@ -525,7 +525,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3871A1D-4416-FE4F-BFE7-11A303AF59C5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -535,6 +535,11 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>